<commit_message>
Ajout gestion semaine 4
</commit_message>
<xml_diff>
--- a/meeting/GestionHedbo_Semaine3.xlsx
+++ b/meeting/GestionHedbo_Semaine3.xlsx
@@ -318,7 +318,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +337,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -588,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -631,41 +637,42 @@
     <xf numFmtId="165" fontId="22" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,17 +976,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -991,9 +998,9 @@
       <c r="A2" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1014,15 +1021,15 @@
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1032,45 +1039,45 @@
       <c r="B5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="21"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="9"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1084,15 +1091,15 @@
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1120,7 +1127,7 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1129,69 +1136,69 @@
       <c r="C12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="23">
+      <c r="D12" s="31"/>
+      <c r="E12" s="24">
         <v>168</v>
       </c>
       <c r="F12" s="13">
         <v>3</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="24">
         <f>E12-SUM(F12:F15)</f>
         <v>158</v>
       </c>
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="23"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="13">
         <v>1</v>
       </c>
-      <c r="G13" s="23"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="14">
         <v>41549</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="23"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="13">
         <v>4</v>
       </c>
-      <c r="G14" s="23"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="14">
         <v>41488</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="23"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="13">
         <v>2</v>
       </c>
-      <c r="G15" s="23"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="24" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -1200,37 +1207,37 @@
       <c r="C16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="23">
+      <c r="D16" s="31"/>
+      <c r="E16" s="24">
         <v>172</v>
       </c>
       <c r="F16" s="13">
         <v>3</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="24">
         <f>(E16-F16)-F17</f>
         <v>160</v>
       </c>
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="14">
         <v>41549</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="23"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="13">
         <v>9</v>
       </c>
-      <c r="G17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="23" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -1239,49 +1246,49 @@
       <c r="C18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="23">
+      <c r="D18" s="31"/>
+      <c r="E18" s="24">
         <v>168</v>
       </c>
       <c r="F18" s="13">
         <v>4</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="23">
         <f>E18-SUM(F18:F20)</f>
         <v>158</v>
       </c>
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="25"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="13">
         <v>3</v>
       </c>
-      <c r="G19" s="24"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="14">
         <v>41488</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="26"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="27"/>
       <c r="F20" s="13">
         <v>3</v>
       </c>
-      <c r="G20" s="23"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1294,7 +1301,7 @@
       <c r="C21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="15">
         <v>168</v>
       </c>
@@ -1308,7 +1315,7 @@
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -1317,37 +1324,37 @@
       <c r="C22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="24">
+      <c r="D22" s="31"/>
+      <c r="E22" s="23">
         <v>176</v>
       </c>
       <c r="F22" s="13">
         <v>4</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="23">
         <f>(E22-F22)-F23</f>
         <v>169</v>
       </c>
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="24"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="13">
         <v>3</v>
       </c>
-      <c r="G23" s="24"/>
+      <c r="G23" s="23"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -1356,33 +1363,33 @@
       <c r="C24" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="24">
+      <c r="D24" s="31"/>
+      <c r="E24" s="23">
         <v>171</v>
       </c>
       <c r="F24" s="13">
         <v>6</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="23">
         <f>(E24-F24)-F25</f>
         <v>163</v>
       </c>
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="24"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="13">
         <v>2</v>
       </c>
-      <c r="G25" s="24"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1395,14 +1402,14 @@
       <c r="C26" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="24">
+      <c r="D26" s="31"/>
+      <c r="E26" s="23">
         <v>168</v>
       </c>
       <c r="F26" s="13">
         <v>10</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="23">
         <f>(E26-F26)-F27</f>
         <v>156</v>
       </c>
@@ -1416,12 +1423,12 @@
       <c r="C27" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="24"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="13">
         <v>2</v>
       </c>
-      <c r="G27" s="24"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1434,11 +1441,11 @@
       <c r="C28" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="31"/>
       <c r="E28" s="11">
         <v>166</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="18">
         <v>3</v>
       </c>
       <c r="G28" s="13">
@@ -1451,10 +1458,10 @@
       <c r="A29" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="28"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="9"/>
       <c r="E29" s="13">
         <v>540</v>
@@ -1467,10 +1474,10 @@
       <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="28"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="9"/>
       <c r="E30" s="13">
         <v>540</v>
@@ -1483,10 +1490,10 @@
       <c r="A31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="28"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="9"/>
       <c r="E31" s="13">
         <v>360</v>
@@ -1499,8 +1506,8 @@
       <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="9"/>
       <c r="E32" s="13">
         <v>1440</v>
@@ -1520,71 +1527,71 @@
       <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="16"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
       <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="22"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
       <c r="H37" s="16"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="22"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="9"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
       <c r="H38" s="16"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
       <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1599,6 +1606,39 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="C37:G37"/>
     <mergeCell ref="C38:G38"/>
@@ -1608,39 +1648,6 @@
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="C35:G36"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>